<commit_message>
Updated Customer Editing Mechanism
</commit_message>
<xml_diff>
--- a/data/Electricity.xlsx
+++ b/data/Electricity.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="April" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="May" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="June" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -624,20 +625,14 @@
           <t>Jane</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="B3" t="n">
+        <v>100</v>
+      </c>
+      <c r="C3" t="n">
+        <v>15</v>
+      </c>
+      <c r="D3" t="n">
+        <v>100</v>
       </c>
       <c r="E3" t="n">
         <v>0.48</v>
@@ -681,6 +676,159 @@
       <c r="H4" t="inlineStr">
         <is>
           <t>May</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Customer Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Consumption Period</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Usage (%)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Consumption Duration</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Net Price</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Month</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2" t="n">
+        <v>50</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>25</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Jane</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>100</v>
+      </c>
+      <c r="C3" t="n">
+        <v>15</v>
+      </c>
+      <c r="D3" t="n">
+        <v>100</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>50</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Jack</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>180</v>
+      </c>
+      <c r="C4" t="n">
+        <v>14</v>
+      </c>
+      <c r="D4" t="n">
+        <v>65</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="F4" t="n">
+        <v>54.98999999999999</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>June</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Admin Privileges to be Service-Wise
</commit_message>
<xml_diff>
--- a/data/Electricity.xlsx
+++ b/data/Electricity.xlsx
@@ -448,12 +448,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Consumption Days</t>
+          <t>Consumption Period</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Usage (%)</t>
+          <t>Utilisation (%)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -558,12 +558,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Consumption Days</t>
+          <t>Consumption Period</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Usage (%)</t>
+          <t>Utilisation (%)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -711,12 +711,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Consumption Days</t>
+          <t>Consumption Period</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Usage (%)</t>
+          <t>Utilisation (%)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">

</xml_diff>